<commit_message>
Push update code 15052024
</commit_message>
<xml_diff>
--- a/New_202306/Missing_Dictionary.xlsx
+++ b/New_202306/Missing_Dictionary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>File_Name</t>
   </si>
@@ -25,19 +25,13 @@
     <t>Flag</t>
   </si>
   <si>
-    <t>IP_Hoa Binh</t>
-  </si>
-  <si>
-    <t>binh phu invest (phu my group)</t>
-  </si>
-  <si>
-    <t>cong ty tnhh hoa phu - hoa binh</t>
-  </si>
-  <si>
-    <t>cong ty cp tap doan phu my</t>
-  </si>
-  <si>
-    <t>Developer</t>
+    <t>IP_BRVT</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>Sub_Type</t>
   </si>
 </sst>
 </file>
@@ -395,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -416,33 +410,16 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last update 17072024 and README.md
</commit_message>
<xml_diff>
--- a/New_202306/Missing_Dictionary.xlsx
+++ b/New_202306/Missing_Dictionary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>File_Name</t>
   </si>
@@ -25,13 +25,13 @@
     <t>Flag</t>
   </si>
   <si>
-    <t>IP_BRVT</t>
-  </si>
-  <si>
-    <t>District</t>
-  </si>
-  <si>
-    <t>Sub_Type</t>
+    <t>IP_Long An</t>
+  </si>
+  <si>
+    <t>slp (sea logistics partners)</t>
+  </si>
+  <si>
+    <t>Developer</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -410,15 +410,10 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>